<commit_message>
update readme and juicerDump2mat fix
</commit_message>
<xml_diff>
--- a/data/indexFiles/sampleMyodTrimDataIndexTp-48_8_80.xlsx
+++ b/data/indexFiles/sampleMyodTrimDataIndexTp-48_8_80.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MATLAB\4DNvestigator\data\indexFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottronquist/projects/4DNvestigator/data/indexFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E677B1B6-3A7D-4023-974C-9AD18D0045BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAEAAA9-5115-D849-A0D8-BE701206A67F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12540" windowHeight="7545" xr2:uid="{29F8AD39-320A-435A-91CF-9AB30172B325}"/>
+    <workbookView xWindow="2660" yWindow="600" windowWidth="25600" windowHeight="14700" xr2:uid="{29F8AD39-320A-435A-91CF-9AB30172B325}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,40 +48,40 @@
     <t>myod</t>
   </si>
   <si>
-    <t>Sample_64585.hic</t>
-  </si>
-  <si>
-    <t>Sample_71530.hic</t>
-  </si>
-  <si>
-    <t>Sample_71531.hic</t>
-  </si>
-  <si>
-    <t>Sample_63246_rsem.genes.results</t>
-  </si>
-  <si>
-    <t>Sample_63247_rsem.genes.results</t>
-  </si>
-  <si>
-    <t>Sample_63248_rsem.genes.results</t>
-  </si>
-  <si>
-    <t>Sample_63249_rsem.genes.results</t>
-  </si>
-  <si>
-    <t>Sample_63250_rsem.genes.results</t>
-  </si>
-  <si>
-    <t>Sample_63251_rsem.genes.results</t>
-  </si>
-  <si>
-    <t>Sample_63273_rsem.genes.results</t>
-  </si>
-  <si>
-    <t>Sample_63274_rsem.genes.results</t>
-  </si>
-  <si>
-    <t>Sample_63275_rsem.genes.results</t>
+    <t>/Users/scottronquist/projects/4DNvestigator/data/projects/myod/raw/rnaseq/Sample_63246_rsem.genes.results</t>
+  </si>
+  <si>
+    <t>/Users/scottronquist/projects/4DNvestigator/data/projects/myod/raw/rnaseq/Sample_63247_rsem.genes.results</t>
+  </si>
+  <si>
+    <t>/Users/scottronquist/projects/4DNvestigator/data/projects/myod/raw/rnaseq/Sample_63248_rsem.genes.results</t>
+  </si>
+  <si>
+    <t>/Users/scottronquist/projects/4DNvestigator/data/projects/myod/raw/rnaseq/Sample_63249_rsem.genes.results</t>
+  </si>
+  <si>
+    <t>/Users/scottronquist/projects/4DNvestigator/data/projects/myod/raw/rnaseq/Sample_63250_rsem.genes.results</t>
+  </si>
+  <si>
+    <t>/Users/scottronquist/projects/4DNvestigator/data/projects/myod/raw/rnaseq/Sample_63273_rsem.genes.results</t>
+  </si>
+  <si>
+    <t>/Users/scottronquist/projects/4DNvestigator/data/projects/myod/raw/rnaseq/Sample_63251_rsem.genes.results</t>
+  </si>
+  <si>
+    <t>/Users/scottronquist/projects/4DNvestigator/data/projects/myod/raw/rnaseq/Sample_63274_rsem.genes.results</t>
+  </si>
+  <si>
+    <t>/Users/scottronquist/projects/4DNvestigator/data/projects/myod/raw/rnaseq/Sample_63275_rsem.genes.results</t>
+  </si>
+  <si>
+    <t>/Users/scottronquist/projects/4DNvestigator/data/projects/myod/raw/hic/Sample_64585_trim.hic</t>
+  </si>
+  <si>
+    <t>/Users/scottronquist/projects/4DNvestigator/data/projects/myod/raw/hic/Sample_71530_trim.hic</t>
+  </si>
+  <si>
+    <t>/Users/scottronquist/projects/4DNvestigator/data/projects/myod/raw/hic/Sample_71531_trim.hic</t>
   </si>
 </sst>
 </file>
@@ -446,18 +446,18 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="153.5" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,9 +471,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -485,9 +485,9 @@
         <v>-48</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -499,9 +499,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -513,9 +513,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -527,9 +527,9 @@
         <v>-48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -541,9 +541,9 @@
         <v>-48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -555,9 +555,9 @@
         <v>-48</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -569,9 +569,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -583,9 +583,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -597,9 +597,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -611,9 +611,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -625,9 +625,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>

</xml_diff>